<commit_message>
parsed right funcding amount
</commit_message>
<xml_diff>
--- a/promega_search_results_response.xlsx
+++ b/promega_search_results_response.xlsx
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Professor of Biochemistry and Molecular Biology, University of British Columbia - ‪‪Cited by 5679‬‬ - ‪Translational control‬ - ‪IRES‬ - ‪positive strand‬ ...</t>
+          <t>Eric Jan. Professor of Biochemistry and Molecular Biology, University of British Columbia. Verified email at mail.ubc.ca - Homepage · Translational ...</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>The Jan Lab. Menu. Research · People · Principal Investigator ... The Life Sciences Institute (LSI) at UBC is the largest Life Sciences Institute in Canada.</t>
+          <t>The Life Sciences Institute (LSI) at UBC is the largest Life Sciences Institute in Canada. Diabetes Research Group. The Jan Lab is located in the Diabetes ...</t>
         </is>
       </c>
     </row>
@@ -589,34 +589,34 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024 Faculty of Medicine Distinguished Achievement Award ...</t>
+          <t>Eric Jan , Co-Founder - NanoVation Therapeutics</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.med.ubc.ca/news/2024-faculty-of-medicine-distinguished-achievement-award-recipients/</t>
+          <t>https://nanovationtx.com/jan-eric-jan-ntx-cofounder/</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Jun 24, 2024 ... Ranked among the world's top medical schools with the fifth-largest MD enrollment in North America, the UBC ... Dr. Eric Jan Biochemistry and ...</t>
+          <t>I am a professor in the Department of Biochemistry and Molecular Biology at UBC. I completed my PhD at Northwestern University and a postdoctoral fellow at ...</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NEB - Freezers</t>
+          <t>2024 Faculty of Medicine Distinguished Achievement Award ...</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.neb.ca/freezer_inventory.php?id=10</t>
+          <t>https://www.med.ubc.ca/news/2024-faculty-of-medicine-distinguished-achievement-award-recipients/</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2350 Health Sciences Mall, Vancouver, British Columbia Freezer Location: Life Sciences Centre Room 5440. On-site Manager: Dr. Eric Jan's Lab</t>
+          <t>Jun 24, 2024 ... Ranked among the world's top medical schools with the fifth-largest MD enrollment in North America, the UBC ... Dr. Eric Jan Biochemistry and ...</t>
         </is>
       </c>
     </row>

</xml_diff>